<commit_message>
Added Dynamic Web Scrap Method
added a better dynamic web scrap method using selenium
</commit_message>
<xml_diff>
--- a/CoinEtoro.xlsx
+++ b/CoinEtoro.xlsx
@@ -424,7 +424,7 @@
     <t>Avalanche</t>
   </si>
   <si>
-    <t xml:space="preserve">Terra 2.0 </t>
+    <t>Terra 2.0</t>
   </si>
   <si>
     <t>Cartesi</t>
@@ -436,7 +436,7 @@
     <t>Universal Market Access</t>
   </si>
   <si>
-    <t xml:space="preserve">Terra Classic </t>
+    <t>Terra Classic</t>
   </si>
   <si>
     <t>FTX Token</t>

</xml_diff>